<commit_message>
create user_input validation.py to be use in creating and exporting events
also fixed other bugs
</commit_message>
<xml_diff>
--- a/Quality/FunctionalTestPlan.xlsx
+++ b/Quality/FunctionalTestPlan.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panuo\OneDrive\Documents\aaSchool_Work\software_engineering\day_flow\Quality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8831ABF-691C-4A82-A78D-10A76116BDF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -249,22 +258,25 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">from 31/1/2023 to </t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
-        <color rgb="FFFF0000"/>
       </rPr>
       <t>31</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t>/2/2023</t>
     </r>
@@ -281,22 +293,25 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">from 30/3/2023 to </t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
-        <color rgb="FFFF0000"/>
       </rPr>
       <t>30</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t>/2/2023</t>
     </r>
@@ -305,39 +320,46 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="mm-dd-yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -363,86 +385,90 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -632,27 +658,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.88"/>
-    <col customWidth="1" min="2" max="2" width="49.5"/>
-    <col customWidth="1" min="3" max="3" width="78.25"/>
-    <col customWidth="1" min="4" max="4" width="33.25"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+    <col min="3" max="3" width="78.21875" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -676,7 +707,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -690,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="19.5" customHeight="1">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -704,7 +735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" ht="19.5" customHeight="1">
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -718,7 +749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" ht="15.0" customHeight="1">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -728,76 +759,82 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="13">
-        <v>43443.0</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="12">
+        <v>43443</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
       <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13">
-        <v>43354.0</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="12">
+        <v>43354</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
       <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
       <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
       <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="D12" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
       <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
@@ -808,62 +845,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="13">
-        <v>43346.0</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="C14" s="12">
+        <v>43346</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="15">
-        <v>43411.0</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="C15" s="14">
+        <v>43411</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
       <c r="B16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="16">
-        <v>43776.0</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="C16" s="15">
+        <v>43776</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
       <c r="B17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" ht="16.5" customHeight="1">
+      <c r="D17" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
       <c r="B18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="D18" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
       <c r="B19" s="8" t="s">
         <v>39</v>
       </c>
@@ -874,7 +917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" ht="15.0" customHeight="1">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>41</v>
       </c>
@@ -884,8 +927,8 @@
       </c>
       <c r="D20" s="10"/>
     </row>
-    <row r="21">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -898,7 +941,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
       <c r="B22" s="8" t="s">
         <v>43</v>
       </c>
@@ -909,8 +953,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -923,7 +967,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
       <c r="B24" s="8" t="s">
         <v>46</v>
       </c>
@@ -934,8 +979,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -948,7 +993,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" ht="16.5" customHeight="1">
+    <row r="26" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
       <c r="B26" s="8" t="s">
         <v>7</v>
       </c>
@@ -959,8 +1005,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="12" t="s">
+    <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -973,7 +1019,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
       <c r="B28" s="8" t="s">
         <v>54</v>
       </c>
@@ -984,7 +1031,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
       <c r="B29" s="8" t="s">
         <v>56</v>
       </c>
@@ -995,7 +1043,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
       <c r="B30" s="8" t="s">
         <v>59</v>
       </c>
@@ -1006,7 +1055,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>62</v>
       </c>
@@ -1016,21 +1065,22 @@
       </c>
       <c r="D31" s="10"/>
     </row>
-    <row r="32">
-      <c r="A32" s="12" t="s">
+    <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
       <c r="B33" s="8" t="s">
         <v>65</v>
       </c>
@@ -1041,8 +1091,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
         <v>67</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1055,7 +1105,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
       <c r="B35" s="8" t="s">
         <v>70</v>
       </c>
@@ -1066,7 +1117,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
       <c r="B36" s="8" t="s">
         <v>43</v>
       </c>
@@ -1077,7 +1129,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
       <c r="B37" s="8" t="s">
         <v>73</v>
       </c>
@@ -1088,15 +1141,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-    </row>
-    <row r="39">
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+    </row>
+    <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>76</v>
       </c>
@@ -1110,15 +1163,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="18" t="s">
+    <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-    </row>
-    <row r="41">
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+    </row>
+    <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>76</v>
       </c>
@@ -1134,17 +1187,16 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A27:A30"/>
     <mergeCell ref="A7:A19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A27:A30"/>
   </mergeCells>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Did some validation testing and fixed code
</commit_message>
<xml_diff>
--- a/Quality/FunctionalTestPlan.xlsx
+++ b/Quality/FunctionalTestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panuo\OneDrive\Documents\aaSchool_Work\software_engineering\day_flow\Quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8831ABF-691C-4A82-A78D-10A76116BDF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794642C3-F789-4291-9FE0-4EAD942CAA5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t>objectives</t>
   </si>
@@ -34,9 +34,6 @@
     <t>expected results</t>
   </si>
   <si>
-    <t>[Search Event]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -88,18 +85,9 @@
     <t xml:space="preserve">One digit day </t>
   </si>
   <si>
-    <t xml:space="preserve">Previous century </t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/04/1920 </t>
-  </si>
-  <si>
     <t>Illegal day</t>
   </si>
   <si>
-    <t xml:space="preserve">31/06/1877 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Leap year </t>
   </si>
   <si>
@@ -145,9 +133,6 @@
     <t>-07/02/2004</t>
   </si>
   <si>
-    <t>[Create Event</t>
-  </si>
-  <si>
     <t>Name Validation</t>
   </si>
   <si>
@@ -214,15 +199,9 @@
     <t>Start date is later than end date</t>
   </si>
   <si>
-    <t>12/10/2023 - 11/9/2023</t>
-  </si>
-  <si>
     <t>No events in the time frame</t>
   </si>
   <si>
-    <t>11/09/2023 - 12/10/2023</t>
-  </si>
-  <si>
     <t>Filename Validation</t>
   </si>
   <si>
@@ -256,76 +235,78 @@
     <t>Next month has lower number of days and the current month</t>
   </si>
   <si>
+    <t>Rejected [Return the last day of the month]</t>
+  </si>
+  <si>
+    <t>[Previous Button]</t>
+  </si>
+  <si>
+    <t>Previous month has lower number of days and the current month</t>
+  </si>
+  <si>
+    <t>[Searc+A2:B24h Event]</t>
+  </si>
+  <si>
+    <t>[Create Event]</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">from 31/1/2023 to </t>
+      <t>from 2023/1/31 to 2023/2/</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>31</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>/2/2023</t>
-    </r>
-  </si>
-  <si>
-    <t>Rejected [Return the last day of the month]</t>
-  </si>
-  <si>
-    <t>[Previous Button]</t>
-  </si>
-  <si>
-    <t>Previous month has lower number of days and the current month</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">from 30/3/2023 to </t>
+      <t>from 2023/3/30 to 2023/2/</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>30</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>/2/2023</t>
-    </r>
+  </si>
+  <si>
+    <t>31-06-1877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>23/02/2023</t>
+  </si>
+  <si>
+    <t>22-04-920</t>
+  </si>
+  <si>
+    <t>Prevoius century</t>
+  </si>
+  <si>
+    <t>2023/10/12 - 2023/9/11</t>
+  </si>
+  <si>
+    <t>2023/09/11 - 2023/10/12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm\-dd\-yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -350,11 +331,38 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +399,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -404,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -425,31 +439,43 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,10 +695,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -683,7 +709,7 @@
     <col min="4" max="4" width="33.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,492 +723,507 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="20">
+        <v>43443</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="12">
-        <v>43443</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="20">
+        <v>43354</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="12">
-        <v>43354</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="8" t="s">
+      <c r="C10" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="8" t="s">
+      <c r="D11" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="8" t="s">
+      <c r="D12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="25">
+        <v>43776</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C13" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="8" t="s">
+      <c r="D13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="25">
+        <v>43776</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C14" s="20">
+        <v>43346</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="C15" s="20">
+        <v>43411</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="8" t="s">
+      <c r="C17" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="12">
-        <v>43346</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="8" t="s">
+      <c r="D17" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="14">
-        <v>43411</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="8" t="s">
+      <c r="C18" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="15">
-        <v>43776</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="8" t="s">
+      <c r="D18" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C19" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="D24" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="D26" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="D27" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="8" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="C28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="D28" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="8" t="s">
+    <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8" t="s">
+      <c r="A32" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="B35" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C35" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="8" t="s">
+      <c r="D35" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D36" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="C37" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="D37" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="D39" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
     </row>
     <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1197,6 +1238,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the functional test plan
</commit_message>
<xml_diff>
--- a/Quality/FunctionalTestPlan.xlsx
+++ b/Quality/FunctionalTestPlan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="212">
   <si>
     <t>Test case ID</t>
   </si>
@@ -332,16 +332,67 @@
     <t>CE-10</t>
   </si>
   <si>
-    <t>Handle recurring event</t>
-  </si>
-  <si>
-    <t>[In the form[...repeat_every="WED"]]</t>
+    <t>Handle general recurring events on the display</t>
+  </si>
+  <si>
+    <t>[In the form[...end after=8] On Daily]</t>
   </si>
   <si>
     <t>Display the event on the weekday of repeat_every “given day”.</t>
   </si>
   <si>
     <t>CE-11</t>
+  </si>
+  <si>
+    <t>Create recurring in create display</t>
+  </si>
+  <si>
+    <t>Handle recurring event [Daily]</t>
+  </si>
+  <si>
+    <t>[In the form[...end after=5] On Daily] and [In the form[...end date=tomorrow date] On Daily]</t>
+  </si>
+  <si>
+    <t>Create event form should update the repeat after and end date correctly</t>
+  </si>
+  <si>
+    <t>CE-12</t>
+  </si>
+  <si>
+    <t>Handle recurring event [Weekly]</t>
+  </si>
+  <si>
+    <t>[In the form[...end after=2] On Weekly]</t>
+  </si>
+  <si>
+    <t>Create event form should disable the end date section</t>
+  </si>
+  <si>
+    <t>CE-13</t>
+  </si>
+  <si>
+    <t>Handle recurring event [Monthly]</t>
+  </si>
+  <si>
+    <t>[In the form[...end after=6] On Monthly]</t>
+  </si>
+  <si>
+    <t>CE-14</t>
+  </si>
+  <si>
+    <t>Handle recurring event [Maximum recurring]</t>
+  </si>
+  <si>
+    <t>[In the form[...end after&gt;9999] On Daily]</t>
+  </si>
+  <si>
+    <t>Create event form on repeat after section should return 9999</t>
+  </si>
+  <si>
+    <t>Create event form on repeat after section should return 10000</t>
+  </si>
+  <si>
+    <t>CE-15</t>
   </si>
   <si>
     <t>Start date is later than end date</t>
@@ -1058,7 +1109,8 @@
     <col customWidth="1" min="2" max="2" width="55.0"/>
     <col customWidth="1" min="3" max="3" width="53.63"/>
     <col customWidth="1" min="4" max="4" width="78.25"/>
-    <col customWidth="1" min="5" max="6" width="47.13"/>
+    <col customWidth="1" min="5" max="5" width="55.38"/>
+    <col customWidth="1" min="6" max="6" width="55.63"/>
     <col customWidth="1" min="7" max="7" width="20.75"/>
     <col customWidth="1" min="8" max="8" width="14.75"/>
   </cols>
@@ -1698,10 +1750,10 @@
       <c r="A31" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="12" t="s">
         <v>107</v>
       </c>
       <c r="E31" s="12" t="s">
@@ -1716,23 +1768,23 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B32" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="11" t="s">
+      <c r="B32" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="C32" s="12" t="s">
         <v>111</v>
       </c>
+      <c r="D32" s="12" t="s">
+        <v>112</v>
+      </c>
       <c r="E32" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>15</v>
@@ -1740,37 +1792,41 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="16"/>
-      <c r="B33" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="A33" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="H33" s="8"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>111</v>
+        <v>118</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>15</v>
@@ -1779,19 +1835,19 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>116</v>
+        <v>121</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>15</v>
@@ -1799,23 +1855,23 @@
       <c r="H35" s="8"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" s="35" t="s">
-        <v>120</v>
+      <c r="A36" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>52</v>
+        <v>127</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>15</v>
@@ -1823,41 +1879,37 @@
       <c r="H36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="A37" s="16"/>
+      <c r="B37" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="34" t="s">
-        <v>126</v>
+        <v>131</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="38" t="s">
         <v>128</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>129</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>15</v>
@@ -1866,19 +1918,19 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>15</v>
@@ -1887,21 +1939,21 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="B40" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G40" s="13" t="s">
@@ -1911,18 +1963,18 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="11" t="s">
         <v>35</v>
       </c>
       <c r="G41" s="13" t="s">
@@ -1932,19 +1984,19 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>15</v>
@@ -1953,19 +2005,19 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>149</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>15</v>
@@ -1974,19 +2026,22 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="34" t="s">
-        <v>146</v>
+        <v>150</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>151</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>149</v>
+        <v>52</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>149</v>
+        <v>52</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>15</v>
@@ -1994,35 +2049,41 @@
       <c r="H44" s="8"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="16"/>
-      <c r="B45" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
+      <c r="A45" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="H45" s="8"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>152</v>
+      <c r="A46" s="34" t="s">
+        <v>157</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>155</v>
+        <v>35</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>15</v>
@@ -2030,20 +2091,20 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="20" t="s">
-        <v>157</v>
+      <c r="A47" s="34" t="s">
+        <v>160</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>160</v>
+        <v>35</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>15</v>
@@ -2051,20 +2112,20 @@
       <c r="H47" s="8"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="20" t="s">
-        <v>161</v>
+      <c r="A48" s="34" t="s">
+        <v>163</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>15</v>
@@ -2073,8 +2134,8 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="16"/>
-      <c r="B49" s="17" t="s">
-        <v>165</v>
+      <c r="B49" s="33" t="s">
+        <v>167</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -2085,22 +2146,22 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>15</v>
@@ -2109,19 +2170,19 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="20" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>15</v>
@@ -2130,143 +2191,217 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F52" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>156</v>
-      </c>
       <c r="G52" s="13" t="s">
         <v>15</v>
       </c>
       <c r="H52" s="8"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="41"/>
-      <c r="B53" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
       <c r="H53" s="8"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-      <c r="M53" s="43"/>
-      <c r="N53" s="43"/>
-      <c r="O53" s="43"/>
-      <c r="P53" s="43"/>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="43"/>
-      <c r="S53" s="43"/>
-      <c r="T53" s="43"/>
-      <c r="U53" s="43"/>
-      <c r="V53" s="43"/>
-      <c r="W53" s="43"/>
-      <c r="X53" s="43"/>
-      <c r="Y53" s="43"/>
-      <c r="Z53" s="43"/>
-      <c r="AA53" s="43"/>
-      <c r="AB53" s="43"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="44" t="s">
+      <c r="A54" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="8"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E55" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="B54" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="C54" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="E54" s="45" t="s">
+      <c r="F55" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="8"/>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="F54" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H54" s="8"/>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B55" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="C55" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="D55" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="E55" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="F55" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H55" s="8"/>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="44" t="s">
-        <v>189</v>
-      </c>
-      <c r="B56" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="C56" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="D56" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="E56" s="45" t="s">
+      <c r="F56" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="8"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="41"/>
+      <c r="B57" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="F56" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="G56" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H56" s="8"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="42"/>
-      <c r="B57" s="42"/>
       <c r="C57" s="42"/>
       <c r="D57" s="42"/>
       <c r="E57" s="42"/>
       <c r="F57" s="42"/>
       <c r="G57" s="42"/>
       <c r="H57" s="8"/>
-    </row>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="43"/>
+      <c r="M57" s="43"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="43"/>
+      <c r="P57" s="43"/>
+      <c r="Q57" s="43"/>
+      <c r="R57" s="43"/>
+      <c r="S57" s="43"/>
+      <c r="T57" s="43"/>
+      <c r="U57" s="43"/>
+      <c r="V57" s="43"/>
+      <c r="W57" s="43"/>
+      <c r="X57" s="43"/>
+      <c r="Y57" s="43"/>
+      <c r="Z57" s="43"/>
+      <c r="AA57" s="43"/>
+      <c r="AB57" s="43"/>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="E58" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="F58" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H58" s="8"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="E59" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="F59" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="8"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="B60" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="F60" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="8"/>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="42"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="8"/>
+    </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1"/>
@@ -3215,19 +3350,24 @@
     <row r="1007" ht="15.75" customHeight="1"/>
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="B46:B48"/>
+  <mergeCells count="12">
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B48"/>
     <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B54:B56"/>
     <mergeCell ref="B8:B20"/>
     <mergeCell ref="H8:H20"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B32:B35"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>